<commit_message>
Reports + ItemCodeDesc Saving Done
Please check the Excel File
</commit_message>
<xml_diff>
--- a/branches/UsamaTasks.xlsx
+++ b/branches/UsamaTasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t>Tasks</t>
   </si>
@@ -133,9 +133,6 @@
   </si>
   <si>
     <t>Completed &amp; Revised</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -529,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,14 +795,19 @@
       <c r="D9" s="5">
         <v>41968</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="5">
+        <v>41974</v>
+      </c>
       <c r="F9" s="6" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="G9" t="s">
         <v>28</v>
       </c>
       <c r="H9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" t="s">
         <v>28</v>
       </c>
       <c r="J9" s="5"/>

</xml_diff>

<commit_message>
Invoice Entry with AutoNumber
</commit_message>
<xml_diff>
--- a/branches/UsamaTasks.xlsx
+++ b/branches/UsamaTasks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="41">
   <si>
     <t>Tasks</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>IssueRet, IssueRetDetail, Item_Sec</t>
+  </si>
+  <si>
+    <t>Sale Order Entry</t>
   </si>
 </sst>
 </file>
@@ -550,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,6 +963,24 @@
       <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="5">
+        <v>41943</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" t="s">
+        <v>28</v>
+      </c>
       <c r="L13" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GateInward with Balloon on SaveEvent
</commit_message>
<xml_diff>
--- a/branches/UsamaTasks.xlsx
+++ b/branches/UsamaTasks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="43">
   <si>
     <t>Tasks</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Change from ASCII to english (For Item Code Des)</t>
+  </si>
+  <si>
+    <t>Ord_Hist, Ord_Det</t>
   </si>
 </sst>
 </file>
@@ -556,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,6 +978,9 @@
       <c r="A13" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="B13" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="C13" s="5">
         <v>41943</v>
       </c>
@@ -985,6 +991,9 @@
         <v>28</v>
       </c>
       <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" t="s">
         <v>28</v>
       </c>
       <c r="J13" t="s">
@@ -995,6 +1004,24 @@
     <row r="14" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>41</v>
+      </c>
+      <c r="C14" s="5">
+        <v>41656</v>
+      </c>
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GateInward with Deletion + Modification in Grid
</commit_message>
<xml_diff>
--- a/branches/UsamaTasks.xlsx
+++ b/branches/UsamaTasks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="44">
   <si>
     <t>Tasks</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Ord_Hist, Ord_Det</t>
+  </si>
+  <si>
+    <t>Deletion in Grid</t>
   </si>
 </sst>
 </file>
@@ -557,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,12 +576,12 @@
     <col min="6" max="6" width="23.28515625" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="28.85546875" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" customWidth="1"/>
-    <col min="12" max="12" width="24.5703125" customWidth="1"/>
+    <col min="9" max="10" width="28.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" customWidth="1"/>
+    <col min="13" max="13" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -607,16 +610,19 @@
         <v>37</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -644,15 +650,15 @@
       <c r="I2" t="s">
         <v>28</v>
       </c>
-      <c r="J2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="4" t="s">
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -683,10 +689,13 @@
       <c r="J3" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="4"/>
-    </row>
-    <row r="4" spans="1:12" ht="39" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" ht="39" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -714,15 +723,15 @@
       <c r="I4" t="s">
         <v>38</v>
       </c>
-      <c r="J4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="4" t="s">
+      <c r="K4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="M4" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -750,13 +759,13 @@
       <c r="I5" t="s">
         <v>28</v>
       </c>
-      <c r="J5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="4"/>
-    </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -784,13 +793,14 @@
       <c r="I6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="4"/>
-    </row>
-    <row r="7" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="9"/>
+      <c r="K6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="5"/>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -803,10 +813,10 @@
       <c r="I7" t="s">
         <v>38</v>
       </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="4"/>
-    </row>
-    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L7" s="5"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -834,13 +844,13 @@
       <c r="I8" t="s">
         <v>28</v>
       </c>
-      <c r="J8" t="s">
-        <v>28</v>
-      </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="4"/>
-    </row>
-    <row r="9" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="5"/>
+      <c r="M8" s="4"/>
+    </row>
+    <row r="9" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -868,13 +878,13 @@
       <c r="I9" t="s">
         <v>28</v>
       </c>
-      <c r="J9" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="4"/>
-    </row>
-    <row r="10" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="5"/>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
@@ -902,13 +912,13 @@
       <c r="I10" t="s">
         <v>28</v>
       </c>
-      <c r="J10" t="s">
-        <v>28</v>
-      </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>31</v>
       </c>
@@ -936,12 +946,12 @@
       <c r="I11" t="s">
         <v>38</v>
       </c>
-      <c r="J11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>33</v>
       </c>
@@ -969,12 +979,12 @@
       <c r="I12" t="s">
         <v>38</v>
       </c>
-      <c r="J12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>40</v>
       </c>
@@ -996,12 +1006,12 @@
       <c r="I13" t="s">
         <v>28</v>
       </c>
-      <c r="J13" t="s">
-        <v>28</v>
-      </c>
-      <c r="L13" s="3"/>
-    </row>
-    <row r="14" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>28</v>
+      </c>
+      <c r="M13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>41</v>
       </c>
@@ -1020,7 +1030,7 @@
       <c r="I14" t="s">
         <v>28</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>